<commit_message>
a bit improved graph
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="53">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -1647,6 +1653,23 @@
         <v>50</v>
       </c>
     </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>